<commit_message>
update some coding and adding some datasets
</commit_message>
<xml_diff>
--- a/Forest/MyForest/Lab Result.xlsx
+++ b/Forest/MyForest/Lab Result.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
   <si>
     <t>数据集</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -151,6 +151,18 @@
 异常判断标准：局部密度估计，而不是用分离的路径作为判断。
 建树结构的思想：基于高斯分布选择随机生成一部分数据，利用这部分数据的特征建立树的结构
 多属性分割的基础：随机生成分离面，用这个分离面计算分离面的阈值，作为左右分支的分离的基础</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>covertype</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shuttle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pima</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -334,13 +346,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -351,12 +369,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -691,21 +703,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="71.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
     </row>
     <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
@@ -831,16 +843,16 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="15">
         <v>1831</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="15">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="15">
         <v>20</v>
       </c>
       <c r="E5" s="3">
@@ -864,18 +876,18 @@
       <c r="K5" s="3">
         <v>0.91600000000000004</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="15">
         <v>0.94</v>
       </c>
-      <c r="M5" s="16">
+      <c r="M5" s="15">
         <v>0.88</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="15"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
       <c r="E6" s="3">
         <v>6</v>
       </c>
@@ -897,20 +909,20 @@
       <c r="K6" s="3">
         <v>0.97199999999999998</v>
       </c>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>5681</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="15">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="15">
         <v>165</v>
       </c>
       <c r="E7" s="3">
@@ -934,18 +946,18 @@
       <c r="K7" s="3">
         <v>0.83199999999999996</v>
       </c>
-      <c r="L7" s="16">
+      <c r="L7" s="15">
         <v>0.64</v>
       </c>
-      <c r="M7" s="16">
+      <c r="M7" s="15">
         <v>0.64</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="15"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="21"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="3">
         <v>6</v>
       </c>
@@ -967,18 +979,18 @@
       <c r="K8" s="3">
         <v>0.86</v>
       </c>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
     </row>
     <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="15"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="3">
         <v>6081</v>
       </c>
       <c r="C9" s="3">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="D9" s="17"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="3">
         <v>6</v>
       </c>
@@ -1049,19 +1061,19 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="15">
         <v>1513</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="15">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="15">
         <v>561</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="15">
         <v>6</v>
       </c>
       <c r="F11" s="3">
@@ -1082,19 +1094,19 @@
       <c r="K11" s="3">
         <v>0.997</v>
       </c>
-      <c r="L11" s="16">
+      <c r="L11" s="15">
         <v>0.998</v>
       </c>
-      <c r="M11" s="16">
+      <c r="M11" s="15">
         <v>0.997</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
       <c r="F12" s="3">
         <v>30</v>
       </c>
@@ -1113,8 +1125,8 @@
       <c r="K12" s="3">
         <v>0.999</v>
       </c>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
     </row>
     <row r="13" spans="1:13" s="10" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
@@ -1389,8 +1401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1409,22 +1421,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="22"/>
     </row>
     <row r="2" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
@@ -1502,7 +1514,9 @@
         <v>0.83599999999999997</v>
       </c>
       <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
+      <c r="L3" s="5">
+        <v>0.68</v>
+      </c>
       <c r="M3" s="5">
         <v>0.75</v>
       </c>
@@ -1595,7 +1609,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="6">
@@ -1604,7 +1618,7 @@
       <c r="C6" s="6">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="15">
         <v>165</v>
       </c>
       <c r="E6" s="5">
@@ -1633,14 +1647,14 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="15"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="5">
         <v>6081</v>
       </c>
       <c r="C7" s="5">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="D7" s="17"/>
+      <c r="D7" s="16"/>
       <c r="E7" s="5">
         <v>6</v>
       </c>
@@ -1879,7 +1893,7 @@
     </row>
     <row r="13" spans="1:14" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B13" s="9">
         <v>768</v>
@@ -1921,7 +1935,7 @@
     </row>
     <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B14" s="14">
         <v>14500</v>
@@ -1960,10 +1974,18 @@
       <c r="N14" s="5"/>
     </row>
     <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="2"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="5">
+        <v>213587</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D15" s="5">
+        <v>11</v>
+      </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -1971,8 +1993,12 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
+      <c r="L15" s="5">
+        <v>0.79</v>
+      </c>
+      <c r="M15" s="5">
+        <v>0.76</v>
+      </c>
       <c r="N15" s="5"/>
     </row>
     <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
@@ -2060,18 +2086,18 @@
       <c r="A1" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="22"/>
     </row>
     <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
@@ -2236,7 +2262,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="7">
@@ -2245,7 +2271,7 @@
       <c r="C6" s="7">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="15">
         <v>165</v>
       </c>
       <c r="E6" s="8">
@@ -2273,14 +2299,14 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="15"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="8">
         <v>6081</v>
       </c>
       <c r="C7" s="8">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="D7" s="17"/>
+      <c r="D7" s="16"/>
       <c r="E7" s="8">
         <v>6</v>
       </c>

</xml_diff>